<commit_message>
2020 Tokyo athlete data
</commit_message>
<xml_diff>
--- a/2020 Data for Medals.xlsx
+++ b/2020 Data for Medals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hema/Desktop/butlerdata/Machine-Learning-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BACA21-141E-FA40-BF3E-89C4F6A19E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E33BF3-10ED-DE43-BBAE-D9E5FC2BA4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{7FEB65AE-3C9B-7F4F-934F-EEB9E4E7E2F6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{7FEB65AE-3C9B-7F4F-934F-EEB9E4E7E2F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Athletes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="220">
   <si>
     <t>No. of Athletes</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Bolivia</t>
   </si>
   <si>
-    <t>Ivory Coast</t>
-  </si>
-  <si>
     <t>San Marino</t>
   </si>
   <si>
@@ -450,9 +447,6 @@
     <t>Maldives</t>
   </si>
   <si>
-    <t>Chinese Taipei</t>
-  </si>
-  <si>
     <t>Cuba</t>
   </si>
   <si>
@@ -643,9 +637,6 @@
   </si>
   <si>
     <t>Gabon</t>
-  </si>
-  <si>
-    <t>North Macedonia</t>
   </si>
   <si>
     <t>Zambia</t>
@@ -1128,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E0A6BB-1666-DC43-9E80-58E1B692B5CF}">
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,9 +1131,9 @@
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1150,9 +1141,8 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1160,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1184,7 +1174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1208,7 +1198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1216,7 +1206,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1224,7 +1214,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1232,7 +1222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1240,7 +1230,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1248,7 +1238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1256,7 +1246,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1264,7 +1254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -1346,7 +1336,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2">
         <v>7</v>
@@ -1354,7 +1344,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="2">
         <v>13</v>
@@ -1362,7 +1352,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2">
         <v>302</v>
@@ -1370,7 +1360,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
@@ -1378,7 +1368,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2">
         <v>2</v>
@@ -1386,7 +1376,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="2">
         <v>42</v>
@@ -1394,7 +1384,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="2">
         <v>7</v>
@@ -1402,7 +1392,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2">
         <v>6</v>
@@ -1410,7 +1400,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34" s="2">
         <v>3</v>
@@ -1418,7 +1408,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35" s="2">
         <v>12</v>
@@ -1426,7 +1416,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2">
         <v>370</v>
@@ -1434,7 +1424,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="2">
         <v>6</v>
@@ -1442,7 +1432,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B38" s="2">
         <v>5</v>
@@ -1450,7 +1440,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="2">
         <v>2</v>
@@ -1458,7 +1448,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="2">
         <v>3</v>
@@ -1466,7 +1456,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B41" s="2">
         <v>57</v>
@@ -1474,7 +1464,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="2">
         <v>406</v>
@@ -1482,47 +1472,47 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B43" s="2">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2">
-        <v>71</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B45" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B46" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>132</v>
+        <v>209</v>
       </c>
       <c r="B47" s="2">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" s="2">
         <v>59</v>
@@ -1530,7 +1520,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B49" s="2">
         <v>68</v>
@@ -1538,7 +1528,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B50" s="2">
         <v>13</v>
@@ -1546,7 +1536,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B51" s="2">
         <v>115</v>
@@ -1554,7 +1544,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B52" s="2">
         <v>7</v>
@@ -1562,7 +1552,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B53" s="2">
         <v>105</v>
@@ -1570,7 +1560,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B54" s="2">
         <v>4</v>
@@ -1578,7 +1568,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B55" s="2">
         <v>2</v>
@@ -1586,7 +1576,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2">
         <v>60</v>
@@ -1594,7 +1584,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" s="2">
         <v>3</v>
@@ -1602,7 +1592,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B58" s="2">
         <v>41</v>
@@ -1610,7 +1600,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B59" s="2">
         <v>133</v>
@@ -1618,7 +1608,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B60" s="2">
         <v>5</v>
@@ -1626,7 +1616,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B61" s="2">
         <v>3</v>
@@ -1634,7 +1624,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B62" s="2">
         <v>13</v>
@@ -1642,7 +1632,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B63" s="2">
         <v>33</v>
@@ -1650,63 +1640,62 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B64" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B65" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B66" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B67" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B68" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B69" s="2">
         <v>398</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B70" s="2">
         <v>5</v>
       </c>
       <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>2</v>
       </c>
@@ -1714,7 +1703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -1722,7 +1711,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>8</v>
       </c>
@@ -1730,7 +1719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>11</v>
       </c>
@@ -1738,7 +1727,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>14</v>
       </c>
@@ -1746,7 +1735,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>17</v>
       </c>
@@ -1754,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>20</v>
       </c>
@@ -1762,7 +1751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>23</v>
       </c>
@@ -1770,7 +1759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>26</v>
       </c>
@@ -1778,7 +1767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>29</v>
       </c>
@@ -1892,63 +1881,63 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B94" s="2">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B95" s="2">
-        <v>50</v>
+        <v>552</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B96" s="2">
-        <v>552</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B97" s="2">
-        <v>14</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B98" s="2">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B99" s="2">
-        <v>85</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B100" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B101" s="2">
         <v>11</v>
@@ -1956,95 +1945,95 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B102" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B103" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B104" s="2">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B105" s="2">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B106" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B107" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B108" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B109" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B110" s="2">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B111" s="2">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="B112" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B113" s="2">
         <v>6</v>
@@ -2052,7 +2041,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B114" s="2">
         <v>5</v>
@@ -2060,7 +2049,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B115" s="2">
         <v>30</v>
@@ -2068,7 +2057,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B116" s="2">
         <v>4</v>
@@ -2076,7 +2065,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B117" s="2">
         <v>4</v>
@@ -2084,7 +2073,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B118" s="2">
         <v>6</v>
@@ -2092,7 +2081,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B119" s="2">
         <v>2</v>
@@ -2100,7 +2089,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B120" s="2">
         <v>2</v>
@@ -2108,7 +2097,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B121" s="2">
         <v>8</v>
@@ -2116,7 +2105,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B122" s="2">
         <v>164</v>
@@ -2124,7 +2113,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B123" s="2">
         <v>19</v>
@@ -2132,7 +2121,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B124" s="2">
         <v>6</v>
@@ -2140,7 +2129,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B125" s="2">
         <v>43</v>
@@ -2148,7 +2137,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B126" s="2">
         <v>34</v>
@@ -2156,7 +2145,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B127" s="2">
         <v>50</v>
@@ -2164,7 +2153,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B128" s="2">
         <v>10</v>
@@ -2172,7 +2161,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B129" s="2">
         <v>3</v>
@@ -2180,7 +2169,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B130" s="2">
         <v>11</v>
@@ -2188,7 +2177,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B131" s="2">
         <v>2</v>
@@ -2196,7 +2185,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B132" s="2">
         <v>5</v>
@@ -2204,7 +2193,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B133" s="2">
         <v>274</v>
@@ -2212,7 +2201,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B134" s="2">
         <v>223</v>
@@ -2220,7 +2209,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B135" s="2">
         <v>8</v>
@@ -2228,7 +2217,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B136" s="2">
         <v>7</v>
@@ -2236,7 +2225,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B137" s="2">
         <v>52</v>
@@ -2244,63 +2233,63 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="B138" s="2">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B139" s="2">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B140" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B141" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B142" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B143" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B144" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B145" s="2">
         <v>8</v>
@@ -2308,215 +2297,215 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B146" s="2">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B147" s="2">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B148" s="2">
-        <v>19</v>
+        <v>210</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B149" s="2">
-        <v>210</v>
+        <v>92</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B150" s="2">
-        <v>92</v>
+        <v>37</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B151" s="2">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B152" s="2">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B153" s="2">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B154" s="2">
-        <v>3</v>
+        <v>101</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>53</v>
+        <v>203</v>
       </c>
       <c r="B155" s="2">
-        <v>101</v>
+        <v>328</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>206</v>
+        <v>56</v>
       </c>
       <c r="B156" s="2">
-        <v>328</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B157" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B158" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B159" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B160" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B161" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B162" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B163" s="2">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B164" s="2">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B165" s="2">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B166" s="2">
-        <v>86</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B167" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B168" s="2">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B169" s="2">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B170" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B171" s="2">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B172" s="2">
         <v>2</v>
@@ -2524,95 +2513,95 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B173" s="2">
-        <v>2</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B174" s="2">
-        <v>177</v>
+        <v>236</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B175" s="2">
-        <v>236</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B176" s="2">
-        <v>2</v>
+        <v>320</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B177" s="2">
-        <v>320</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B178" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B179" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B180" s="2">
-        <v>3</v>
+        <v>134</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B181" s="2">
-        <v>134</v>
+        <v>106</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B182" s="2">
-        <v>106</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="B183" s="2">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B184" s="2">
         <v>11</v>
@@ -2620,7 +2609,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B185" s="2">
         <v>3</v>
@@ -2628,7 +2617,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B186" s="2">
         <v>42</v>
@@ -2636,7 +2625,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B187" s="2">
         <v>4</v>
@@ -2644,7 +2633,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B188" s="2">
         <v>4</v>
@@ -2652,7 +2641,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B189" s="2">
         <v>6</v>
@@ -2660,7 +2649,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B190" s="2">
         <v>22</v>
@@ -2668,7 +2657,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B191" s="2">
         <v>63</v>
@@ -2676,7 +2665,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B192" s="2">
         <v>108</v>
@@ -2684,7 +2673,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B193" s="2">
         <v>9</v>
@@ -2692,7 +2681,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B194" s="2">
         <v>2</v>
@@ -2700,7 +2689,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B195" s="2">
         <v>21</v>
@@ -2708,7 +2697,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B196" s="2">
         <v>155</v>
@@ -2716,7 +2705,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B197" s="2">
         <v>5</v>
@@ -2724,7 +2713,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B198" s="2">
         <v>613</v>
@@ -2732,7 +2721,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B199" s="2">
         <v>11</v>
@@ -2740,7 +2729,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B200" s="2">
         <v>63</v>
@@ -2748,7 +2737,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B201" s="2">
         <v>3</v>
@@ -2756,7 +2745,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B202" s="2">
         <v>44</v>
@@ -2764,7 +2753,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B203" s="2">
         <v>18</v>
@@ -2772,7 +2761,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B204" s="2">
         <v>4</v>
@@ -2780,7 +2769,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B205" s="2">
         <v>5</v>
@@ -2788,7 +2777,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B206" s="2">
         <v>24</v>
@@ -2796,14 +2785,14 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B207" s="2">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B207">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F207">
     <sortCondition ref="A2:A207"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2814,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31B0A23-9814-D045-9163-D5049203E195}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C94"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A94" sqref="A2:A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2826,13 +2815,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2947,7 +2936,7 @@
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5">
         <v>2351627</v>
@@ -2958,7 +2947,7 @@
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="5">
         <v>212559417</v>
@@ -2969,7 +2958,7 @@
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="5">
         <v>6948445</v>
@@ -2980,7 +2969,7 @@
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="5">
         <v>20903273</v>
@@ -2991,7 +2980,7 @@
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5">
         <v>37742154</v>
@@ -3002,7 +2991,7 @@
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="5">
         <v>1439323776</v>
@@ -3013,7 +3002,7 @@
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="5">
         <v>50882891</v>
@@ -3024,7 +3013,7 @@
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B19" s="5">
         <v>26378274</v>
@@ -3035,7 +3024,7 @@
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="5">
         <v>4105267</v>
@@ -3046,7 +3035,7 @@
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B21" s="5">
         <v>11326616</v>
@@ -3057,7 +3046,7 @@
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B22" s="5">
         <v>10551219</v>
@@ -3068,7 +3057,7 @@
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B23" s="5">
         <v>5792202</v>
@@ -3079,7 +3068,7 @@
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B24" s="5">
         <v>10847910</v>
@@ -3090,7 +3079,7 @@
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B25" s="5">
         <v>17643054</v>
@@ -3101,7 +3090,7 @@
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B26" s="5">
         <v>102334404</v>
@@ -3112,7 +3101,7 @@
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B27" s="5">
         <v>1326535</v>
@@ -3123,7 +3112,7 @@
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B28" s="5">
         <v>114963588</v>
@@ -3134,7 +3123,7 @@
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B29" s="5">
         <v>896445</v>
@@ -3145,7 +3134,7 @@
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B30" s="5">
         <v>5540720</v>
@@ -3156,7 +3145,7 @@
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B31" s="5">
         <v>65273511</v>
@@ -3321,7 +3310,7 @@
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="5">
         <v>2961167</v>
@@ -3332,7 +3321,7 @@
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="5">
         <v>126476461</v>
@@ -3343,7 +3332,7 @@
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5">
         <v>10203134</v>
@@ -3354,7 +3343,7 @@
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5">
         <v>18776707</v>
@@ -3365,7 +3354,7 @@
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="5">
         <v>53771296</v>
@@ -3376,7 +3365,7 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5">
         <v>1859203</v>
@@ -3387,7 +3376,7 @@
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B52" s="5">
         <v>4270571</v>
@@ -3398,7 +3387,7 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="5">
         <v>6524195</v>
@@ -3409,7 +3398,7 @@
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="5">
         <v>1886198</v>
@@ -3420,7 +3409,7 @@
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B55" s="5">
         <v>2722289</v>
@@ -3431,7 +3420,7 @@
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B56" s="5">
         <v>2078453</v>
@@ -3442,7 +3431,7 @@
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B57" s="5">
         <v>32365999</v>
@@ -3453,7 +3442,7 @@
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B58" s="5">
         <v>128932753</v>
@@ -3464,7 +3453,7 @@
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B59" s="5">
         <v>4033963</v>
@@ -3475,7 +3464,7 @@
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B60" s="5">
         <v>3278290</v>
@@ -3486,7 +3475,7 @@
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B61" s="5">
         <v>36910560</v>
@@ -3497,7 +3486,7 @@
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B62" s="5">
         <v>2540905</v>
@@ -3508,7 +3497,7 @@
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B63" s="5">
         <v>17134872</v>
@@ -3519,7 +3508,7 @@
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B64" s="5">
         <v>4822233</v>
@@ -3530,7 +3519,7 @@
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B65" s="5">
         <v>206139589</v>
@@ -3618,7 +3607,7 @@
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B73" s="5">
         <v>144096812</v>
@@ -3629,7 +3618,7 @@
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="5">
         <v>33931</v>
@@ -3640,7 +3629,7 @@
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="5">
         <v>34813871</v>
@@ -3651,7 +3640,7 @@
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B76" s="5">
         <v>8737371</v>
@@ -3662,7 +3651,7 @@
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" s="5">
         <v>5459642</v>
@@ -3673,7 +3662,7 @@
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78" s="5">
         <v>2078938</v>
@@ -3684,7 +3673,7 @@
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B79" s="5">
         <v>59308690</v>
@@ -3695,7 +3684,7 @@
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B80" s="5">
         <v>51269185</v>
@@ -3706,7 +3695,7 @@
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B81" s="5">
         <v>46754778</v>
@@ -3717,7 +3706,7 @@
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B82" s="5">
         <v>10099265</v>
@@ -3728,7 +3717,7 @@
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B83" s="5">
         <v>8654622</v>
@@ -3739,7 +3728,7 @@
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B84" s="5">
         <v>18502413</v>
@@ -3750,7 +3739,7 @@
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B85" s="5">
         <v>23510000</v>
@@ -3761,7 +3750,7 @@
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B86" s="5">
         <v>69799978</v>
@@ -3772,7 +3761,7 @@
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B87" s="5">
         <v>11818619</v>
@@ -3783,7 +3772,7 @@
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B88" s="5">
         <v>84339067</v>
@@ -3794,7 +3783,7 @@
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B89" s="5">
         <v>6031200</v>
@@ -3805,7 +3794,7 @@
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B90" s="5">
         <v>45741007</v>
@@ -3816,7 +3805,7 @@
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B91" s="5">
         <v>43733762</v>
@@ -3827,7 +3816,7 @@
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B92" s="5">
         <v>331002651</v>
@@ -3838,7 +3827,7 @@
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B93" s="5">
         <v>33469203</v>
@@ -3849,7 +3838,7 @@
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B94" s="5">
         <v>31108083</v>
@@ -3870,7 +3859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407E063B-465F-FF4D-B4FF-4ABE654D1EB2}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A66" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -3882,28 +3871,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" t="s">
         <v>218</v>
       </c>
-      <c r="F1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1" t="s">
-        <v>221</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3926,7 +3915,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="4">
-        <f>SUM(D2:F2)</f>
+        <f t="shared" ref="G2:G33" si="0">SUM(D2:F2)</f>
         <v>3</v>
       </c>
       <c r="H2" s="5">
@@ -3956,7 +3945,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="4">
-        <f>SUM(D3:F3)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H3" s="5">
@@ -3986,7 +3975,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="4">
-        <f>SUM(D4:F4)</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="H4" s="5">
@@ -4016,7 +4005,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="4">
-        <f>SUM(D5:F5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H5" s="5">
@@ -4046,7 +4035,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="4">
-        <f>SUM(D6:F6)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H6" s="5">
@@ -4076,7 +4065,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <f>SUM(D7:F7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H7" s="5">
@@ -4106,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="4">
-        <f>SUM(D8:F8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H8" s="5">
@@ -4136,7 +4125,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="4">
-        <f>SUM(D9:F9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H9" s="5">
@@ -4166,7 +4155,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="4">
-        <f>SUM(D10:F10)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H10" s="5">
@@ -4196,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <f>SUM(D11:F11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H11" s="5">
@@ -4211,7 +4200,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4">
         <v>2020</v>
@@ -4226,7 +4215,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <f>SUM(D12:F12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H12" s="5">
@@ -4241,7 +4230,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4">
         <v>2020</v>
@@ -4256,7 +4245,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="4">
-        <f>SUM(D13:F13)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="H13" s="5">
@@ -4271,7 +4260,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="4">
         <v>2020</v>
@@ -4286,7 +4275,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="4">
-        <f>SUM(D14:F14)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H14" s="5">
@@ -4301,7 +4290,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="4">
         <v>2020</v>
@@ -4316,7 +4305,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="4">
-        <f>SUM(D15:F15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H15" s="5">
@@ -4331,7 +4320,7 @@
         <v>66</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4">
         <v>2020</v>
@@ -4346,7 +4335,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="4">
-        <f>SUM(D16:F16)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="H16" s="5">
@@ -4361,7 +4350,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="4">
         <v>2020</v>
@@ -4376,7 +4365,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="4">
-        <f>SUM(D17:F17)</f>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="H17" s="5">
@@ -4391,7 +4380,7 @@
         <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" s="4">
         <v>2020</v>
@@ -4406,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="4">
-        <f>SUM(D18:F18)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H18" s="5">
@@ -4421,7 +4410,7 @@
         <v>73</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C19" s="4">
         <v>2020</v>
@@ -4436,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="4">
-        <f>SUM(D19:F19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H19" s="5">
@@ -4451,7 +4440,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="4">
         <v>2020</v>
@@ -4466,7 +4455,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="4">
-        <f>SUM(D20:F20)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H20" s="5">
@@ -4481,7 +4470,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" s="4">
         <v>2020</v>
@@ -4496,7 +4485,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="4">
-        <f>SUM(D21:F21)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="H21" s="5">
@@ -4511,7 +4500,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" s="4">
         <v>2020</v>
@@ -4526,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="4">
-        <f>SUM(D22:F22)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H22" s="5">
@@ -4541,7 +4530,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C23" s="4">
         <v>2020</v>
@@ -4556,7 +4545,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="4">
-        <f>SUM(D23:F23)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H23" s="5">
@@ -4571,7 +4560,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C24" s="4">
         <v>2020</v>
@@ -4586,7 +4575,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="4">
-        <f>SUM(D24:F24)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H24" s="5">
@@ -4601,7 +4590,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C25" s="4">
         <v>2020</v>
@@ -4616,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f>SUM(D25:F25)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H25" s="5">
@@ -4631,7 +4620,7 @@
         <v>55</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C26" s="4">
         <v>2020</v>
@@ -4646,7 +4635,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="4">
-        <f>SUM(D26:F26)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H26" s="5">
@@ -4661,7 +4650,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C27" s="4">
         <v>2020</v>
@@ -4676,7 +4665,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="4">
-        <f>SUM(D27:F27)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H27" s="5">
@@ -4691,7 +4680,7 @@
         <v>33</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C28" s="4">
         <v>2020</v>
@@ -4706,7 +4695,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="4">
-        <f>SUM(D28:F28)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H28" s="5">
@@ -4721,7 +4710,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C29" s="4">
         <v>2020</v>
@@ -4736,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="4">
-        <f>SUM(D29:F29)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H29" s="5">
@@ -4751,7 +4740,7 @@
         <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C30" s="4">
         <v>2020</v>
@@ -4766,7 +4755,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="4">
-        <f>SUM(D30:F30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H30" s="5">
@@ -4781,7 +4770,7 @@
         <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C31" s="4">
         <v>2020</v>
@@ -4796,7 +4785,7 @@
         <v>11</v>
       </c>
       <c r="G31" s="4">
-        <f>SUM(D31:F31)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="H31" s="5">
@@ -4826,7 +4815,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="4">
-        <f>SUM(D32:F32)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H32" s="5">
@@ -4856,7 +4845,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="4">
-        <f>SUM(D33:F33)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="H33" s="5">
@@ -4886,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="4">
-        <f>SUM(D34:F34)</f>
+        <f t="shared" ref="G34:G65" si="1">SUM(D34:F34)</f>
         <v>1</v>
       </c>
       <c r="H34" s="5">
@@ -4916,7 +4905,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="4">
-        <f>SUM(D35:F35)</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="H35" s="5">
@@ -4946,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="4">
-        <f>SUM(D36:F36)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H36" s="5">
@@ -4976,7 +4965,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="4">
-        <f>SUM(D37:F37)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H37" s="5">
@@ -5006,7 +4995,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="4">
-        <f>SUM(D38:F38)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="H38" s="5">
@@ -5036,7 +5025,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="4">
-        <f>SUM(D39:F39)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H39" s="5">
@@ -5066,7 +5055,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="4">
-        <f>SUM(D40:F40)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H40" s="5">
@@ -5096,7 +5085,7 @@
         <v>3</v>
       </c>
       <c r="G41" s="4">
-        <f>SUM(D41:F41)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H41" s="5">
@@ -5126,7 +5115,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="4">
-        <f>SUM(D42:F42)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H42" s="5">
@@ -5156,7 +5145,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="4">
-        <f>SUM(D43:F43)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H43" s="5">
@@ -5186,7 +5175,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="4">
-        <f>SUM(D44:F44)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H44" s="5">
@@ -5216,7 +5205,7 @@
         <v>20</v>
       </c>
       <c r="G45" s="4">
-        <f>SUM(D45:F45)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="H45" s="5">
@@ -5231,7 +5220,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="4">
         <v>2020</v>
@@ -5246,7 +5235,7 @@
         <v>4</v>
       </c>
       <c r="G46" s="4">
-        <f>SUM(D46:F46)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="H46" s="5">
@@ -5261,7 +5250,7 @@
         <v>65</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" s="4">
         <v>2020</v>
@@ -5276,7 +5265,7 @@
         <v>17</v>
       </c>
       <c r="G47" s="4">
-        <f>SUM(D47:F47)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H47" s="5">
@@ -5291,7 +5280,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="4">
         <v>2020</v>
@@ -5306,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="4">
-        <f>SUM(D48:F48)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H48" s="5">
@@ -5321,7 +5310,7 @@
         <v>50</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="4">
         <v>2020</v>
@@ -5336,7 +5325,7 @@
         <v>8</v>
       </c>
       <c r="G49" s="4">
-        <f>SUM(D49:F49)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H49" s="5">
@@ -5351,7 +5340,7 @@
         <v>16</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="4">
         <v>2020</v>
@@ -5366,7 +5355,7 @@
         <v>2</v>
       </c>
       <c r="G50" s="4">
-        <f>SUM(D50:F50)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H50" s="5">
@@ -5381,7 +5370,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" s="4">
         <v>2020</v>
@@ -5396,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="4">
-        <f>SUM(D51:F51)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H51" s="5">
@@ -5411,7 +5400,7 @@
         <v>87</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" s="4">
         <v>2020</v>
@@ -5426,7 +5415,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="4">
-        <f>SUM(D52:F52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H52" s="5">
@@ -5441,7 +5430,7 @@
         <v>6</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="4">
         <v>2020</v>
@@ -5456,7 +5445,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="4">
-        <f>SUM(D53:F53)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H53" s="5">
@@ -5471,7 +5460,7 @@
         <v>27</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" s="4">
         <v>2020</v>
@@ -5486,7 +5475,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="4">
-        <f>SUM(D54:F54)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H54" s="5">
@@ -5501,7 +5490,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" s="4">
         <v>2020</v>
@@ -5516,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="4">
-        <f>SUM(D55:F55)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H55" s="5">
@@ -5531,7 +5520,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C56" s="4">
         <v>2020</v>
@@ -5546,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="4">
-        <f>SUM(D56:F56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H56" s="5">
@@ -5561,7 +5550,7 @@
         <v>85</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="4">
         <v>2020</v>
@@ -5576,7 +5565,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4">
-        <f>SUM(D57:F57)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H57" s="5">
@@ -5591,7 +5580,7 @@
         <v>92</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C58" s="4">
         <v>2020</v>
@@ -5606,7 +5595,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="4">
-        <f>SUM(D58:F58)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H58" s="5">
@@ -5621,7 +5610,7 @@
         <v>31</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C59" s="4">
         <v>2020</v>
@@ -5636,7 +5625,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="4">
-        <f>SUM(D59:F59)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H59" s="5">
@@ -5651,7 +5640,7 @@
         <v>11</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C60" s="4">
         <v>2020</v>
@@ -5666,7 +5655,7 @@
         <v>3</v>
       </c>
       <c r="G60" s="4">
-        <f>SUM(D60:F60)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H60" s="5">
@@ -5681,7 +5670,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C61" s="4">
         <v>2020</v>
@@ -5696,7 +5685,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="4">
-        <f>SUM(D61:F61)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H61" s="5">
@@ -5711,7 +5700,7 @@
         <v>28</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C62" s="4">
         <v>2020</v>
@@ -5726,7 +5715,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="4">
-        <f>SUM(D62:F62)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H62" s="5">
@@ -5741,7 +5730,7 @@
         <v>36</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C63" s="4">
         <v>2020</v>
@@ -5756,7 +5745,7 @@
         <v>14</v>
       </c>
       <c r="G63" s="4">
-        <f>SUM(D63:F63)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="H63" s="5">
@@ -5771,7 +5760,7 @@
         <v>24</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C64" s="4">
         <v>2020</v>
@@ -5786,7 +5775,7 @@
         <v>7</v>
       </c>
       <c r="G64" s="4">
-        <f>SUM(D64:F64)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H64" s="5">
@@ -5801,7 +5790,7 @@
         <v>88</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C65" s="4">
         <v>2020</v>
@@ -5816,7 +5805,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="4">
-        <f>SUM(D65:F65)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H65" s="5">
@@ -5846,7 +5835,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="4">
-        <f>SUM(D66:F66)</f>
+        <f t="shared" ref="G66:G97" si="2">SUM(D66:F66)</f>
         <v>8</v>
       </c>
       <c r="H66" s="5">
@@ -5876,7 +5865,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="4">
-        <f>SUM(D67:F67)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H67" s="5">
@@ -5906,7 +5895,7 @@
         <v>5</v>
       </c>
       <c r="G68" s="4">
-        <f>SUM(D68:F68)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="H68" s="5">
@@ -5936,7 +5925,7 @@
         <v>2</v>
       </c>
       <c r="G69" s="4">
-        <f>SUM(D69:F69)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H69" s="5">
@@ -5966,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="4">
-        <f>SUM(D70:F70)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H70" s="5">
@@ -5996,7 +5985,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="4">
-        <f>SUM(D71:F71)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H71" s="5">
@@ -6026,7 +6015,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="4">
-        <f>SUM(D72:F72)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H72" s="5">
@@ -6041,7 +6030,7 @@
         <v>37</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C73" s="4">
         <v>2020</v>
@@ -6056,7 +6045,7 @@
         <v>23</v>
       </c>
       <c r="G73" s="4">
-        <f>SUM(D73:F73)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="H73" s="5">
@@ -6071,7 +6060,7 @@
         <v>1</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C74" s="4">
         <v>2020</v>
@@ -6086,7 +6075,7 @@
         <v>2</v>
       </c>
       <c r="G74" s="4">
-        <f>SUM(D74:F74)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H74" s="5">
@@ -6101,7 +6090,7 @@
         <v>93</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" s="4">
         <v>2020</v>
@@ -6116,7 +6105,7 @@
         <v>0</v>
       </c>
       <c r="G75" s="4">
-        <f>SUM(D75:F75)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H75" s="5">
@@ -6131,7 +6120,7 @@
         <v>10</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C76" s="4">
         <v>2020</v>
@@ -6146,7 +6135,7 @@
         <v>5</v>
       </c>
       <c r="G76" s="4">
-        <f>SUM(D76:F76)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H76" s="5">
@@ -6161,7 +6150,7 @@
         <v>35</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="4">
         <v>2020</v>
@@ -6176,7 +6165,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="4">
-        <f>SUM(D77:F77)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H77" s="5">
@@ -6191,7 +6180,7 @@
         <v>18</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="4">
         <v>2020</v>
@@ -6206,7 +6195,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="4">
-        <f>SUM(D78:F78)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="H78" s="5">
@@ -6221,7 +6210,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C79" s="4">
         <v>2020</v>
@@ -6236,7 +6225,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="4">
-        <f>SUM(D79:F79)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H79" s="5">
@@ -6251,7 +6240,7 @@
         <v>72</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C80" s="4">
         <v>2020</v>
@@ -6266,7 +6255,7 @@
         <v>10</v>
       </c>
       <c r="G80" s="4">
-        <f>SUM(D80:F80)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="H80" s="5">
@@ -6281,7 +6270,7 @@
         <v>75</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C81" s="4">
         <v>2020</v>
@@ -6296,7 +6285,7 @@
         <v>6</v>
       </c>
       <c r="G81" s="4">
-        <f>SUM(D81:F81)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="H81" s="5">
@@ -6311,7 +6300,7 @@
         <v>53</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C82" s="4">
         <v>2020</v>
@@ -6326,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="G82" s="4">
-        <f>SUM(D82:F82)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H82" s="5">
@@ -6341,7 +6330,7 @@
         <v>59</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C83" s="4">
         <v>2020</v>
@@ -6356,7 +6345,7 @@
         <v>6</v>
       </c>
       <c r="G83" s="4">
-        <f>SUM(D83:F83)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="H83" s="5">
@@ -6371,7 +6360,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84" s="4">
         <v>2020</v>
@@ -6386,7 +6375,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="4">
-        <f>SUM(D84:F84)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H84" s="5">
@@ -6401,7 +6390,7 @@
         <v>51</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C85" s="4">
         <v>2020</v>
@@ -6416,7 +6405,7 @@
         <v>6</v>
       </c>
       <c r="G85" s="4">
-        <f>SUM(D85:F85)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="H85" s="5">
@@ -6431,7 +6420,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C86" s="4">
         <v>2020</v>
@@ -6446,7 +6435,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="4">
-        <f>SUM(D86:F86)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H86" s="5">
@@ -6461,7 +6450,7 @@
         <v>29</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C87" s="4">
         <v>2020</v>
@@ -6476,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="G87" s="4">
-        <f>SUM(D87:F87)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H87" s="5">
@@ -6491,7 +6480,7 @@
         <v>76</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C88" s="4">
         <v>2020</v>
@@ -6506,7 +6495,7 @@
         <v>9</v>
       </c>
       <c r="G88" s="4">
-        <f>SUM(D88:F88)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="H88" s="5">
@@ -6521,7 +6510,7 @@
         <v>49</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C89" s="4">
         <v>2020</v>
@@ -6536,7 +6525,7 @@
         <v>0</v>
       </c>
       <c r="G89" s="4">
-        <f>SUM(D89:F89)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H89" s="5">
@@ -6551,7 +6540,7 @@
         <v>13</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C90" s="4">
         <v>2020</v>
@@ -6566,7 +6555,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="4">
-        <f>SUM(D90:F90)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H90" s="5">
@@ -6581,7 +6570,7 @@
         <v>21</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C91" s="4">
         <v>2020</v>
@@ -6596,7 +6585,7 @@
         <v>12</v>
       </c>
       <c r="G91" s="4">
-        <f>SUM(D91:F91)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="H91" s="5">
@@ -6611,7 +6600,7 @@
         <v>83</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C92" s="4">
         <v>2020</v>
@@ -6626,7 +6615,7 @@
         <v>33</v>
       </c>
       <c r="G92" s="4">
-        <f>SUM(D92:F92)</f>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="H92" s="5">
@@ -6641,7 +6630,7 @@
         <v>19</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C93" s="4">
         <v>2020</v>
@@ -6656,7 +6645,7 @@
         <v>2</v>
       </c>
       <c r="G93" s="4">
-        <f>SUM(D93:F93)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="H93" s="5">
@@ -6671,7 +6660,7 @@
         <v>64</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C94" s="4">
         <v>2020</v>
@@ -6686,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="G94" s="4">
-        <f>SUM(D94:F94)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H94" s="5">
@@ -6720,16 +6709,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6863,7 +6852,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4">
         <v>17.41</v>
@@ -6875,7 +6864,7 @@
         <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4">
         <v>2053.59</v>
@@ -6887,7 +6876,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="4">
         <v>58.22</v>
@@ -6899,7 +6888,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="4">
         <v>12.32</v>
@@ -6911,7 +6900,7 @@
         <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="4">
         <v>1647.12</v>
@@ -6923,7 +6912,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="4">
         <v>12237.7</v>
@@ -6935,7 +6924,7 @@
         <v>70</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="4">
         <v>314.45999999999998</v>
@@ -6947,7 +6936,7 @@
         <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C20" s="4">
         <v>37.35</v>
@@ -6959,7 +6948,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="4">
         <v>55.21</v>
@@ -6971,7 +6960,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22" s="4">
         <v>96.85</v>
@@ -6983,7 +6972,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23" s="4">
         <v>215.22</v>
@@ -6995,7 +6984,7 @@
         <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24" s="4">
         <v>329.87</v>
@@ -7007,7 +6996,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" s="4">
         <v>75.930000000000007</v>
@@ -7019,7 +7008,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C26" s="4">
         <v>104.3</v>
@@ -7031,7 +7020,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C27" s="4">
         <v>235.37</v>
@@ -7043,7 +7032,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C28" s="4">
         <v>26.61</v>
@@ -7055,7 +7044,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C29" s="4">
         <v>80.56</v>
@@ -7067,7 +7056,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C30" s="4">
         <v>5.0599999999999996</v>
@@ -7079,7 +7068,7 @@
         <v>89</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C31" s="4">
         <v>252.3</v>
@@ -7091,7 +7080,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C32" s="4">
         <v>2582.5</v>
@@ -7271,7 +7260,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="4">
         <v>14.78</v>
@@ -7283,7 +7272,7 @@
         <v>65</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" s="4">
         <v>4872.42</v>
@@ -7295,7 +7284,7 @@
         <v>40</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" s="4">
         <v>40.07</v>
@@ -7307,7 +7296,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="4">
         <v>162.88999999999999</v>
@@ -7319,7 +7308,7 @@
         <v>16</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" s="4">
         <v>79.260000000000005</v>
@@ -7331,7 +7320,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C52" s="4">
         <v>18.84</v>
@@ -7343,7 +7332,7 @@
         <v>87</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="4">
         <v>120.13</v>
@@ -7355,7 +7344,7 @@
         <v>6</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" s="4">
         <v>7.56</v>
@@ -7367,7 +7356,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="4">
         <v>30.46</v>
@@ -7379,7 +7368,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C56" s="4">
         <v>47.54</v>
@@ -7391,7 +7380,7 @@
         <v>25</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C57" s="4">
         <v>10.17</v>
@@ -7403,7 +7392,7 @@
         <v>85</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" s="4">
         <v>314.70999999999998</v>
@@ -7415,7 +7404,7 @@
         <v>92</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59" s="4">
         <v>1150.8900000000001</v>
@@ -7427,7 +7416,7 @@
         <v>31</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C60" s="4">
         <v>8.1300000000000008</v>
@@ -7439,7 +7428,7 @@
         <v>11</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C61" s="4">
         <v>11.43</v>
@@ -7451,7 +7440,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C62" s="4">
         <v>109.71</v>
@@ -7463,7 +7452,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C63" s="4">
         <v>13.25</v>
@@ -7475,7 +7464,7 @@
         <v>36</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C64" s="4">
         <v>830.57</v>
@@ -7487,7 +7476,7 @@
         <v>24</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C65" s="4">
         <v>204.14</v>
@@ -7499,7 +7488,7 @@
         <v>88</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C66" s="4">
         <v>375.75</v>
@@ -7595,7 +7584,7 @@
         <v>37</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C74" s="4">
         <v>1857.77</v>
@@ -7607,7 +7596,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C75" s="4">
         <v>1.63</v>
@@ -7619,7 +7608,7 @@
         <v>93</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C76" s="4">
         <v>686.74</v>
@@ -7631,7 +7620,7 @@
         <v>10</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C77" s="4">
         <v>41.43</v>
@@ -7643,7 +7632,7 @@
         <v>35</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" s="4">
         <v>95.62</v>
@@ -7655,7 +7644,7 @@
         <v>18</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" s="4">
         <v>48.77</v>
@@ -7667,7 +7656,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C80" s="4">
         <v>348.87</v>
@@ -7679,7 +7668,7 @@
         <v>72</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" s="4">
         <v>1530.75</v>
@@ -7691,7 +7680,7 @@
         <v>75</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C82" s="4">
         <v>1314.31</v>
@@ -7703,7 +7692,7 @@
         <v>53</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C83" s="4">
         <v>535.61</v>
@@ -7715,7 +7704,7 @@
         <v>59</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C84" s="4">
         <v>678.97</v>
@@ -7727,7 +7716,7 @@
         <v>81</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C85" s="4">
         <v>52.58</v>
@@ -7739,7 +7728,7 @@
         <v>51</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C86" s="4">
         <v>466</v>
@@ -7751,7 +7740,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C87" s="4">
         <v>455.3</v>
@@ -7763,7 +7752,7 @@
         <v>29</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C88" s="4">
         <v>39.950000000000003</v>
@@ -7775,7 +7764,7 @@
         <v>76</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C89" s="4">
         <v>851.55</v>
@@ -7787,7 +7776,7 @@
         <v>49</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C90" s="4">
         <v>37.93</v>
@@ -7799,7 +7788,7 @@
         <v>13</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C91" s="4">
         <v>26</v>
@@ -7811,7 +7800,7 @@
         <v>21</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C92" s="4">
         <v>112.15</v>
@@ -7823,7 +7812,7 @@
         <v>83</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C93" s="4">
         <v>19485.39</v>
@@ -7835,7 +7824,7 @@
         <v>19</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C94" s="4">
         <v>49.68</v>
@@ -7847,7 +7836,7 @@
         <v>64</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C95" s="4">
         <v>316.48</v>

</xml_diff>